<commit_message>
Databases for Power Generation and GDP/Population
</commit_message>
<xml_diff>
--- a/Data/WindPotential/Philippine_regions_windpotential.xlsx
+++ b/Data/WindPotential/Philippine_regions_windpotential.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upsystem-my.sharepoint.com/personal/rechavez_outlook_up_edu_ph/Documents/1 - EDUCATION/SCHOOLWORK/Undergraduate/Semester 6/CS 132/Machine Project/Solar-Wind-Energy-Analysis-Philippines/Data/SolarPotential/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upsystem-my.sharepoint.com/personal/rechavez_outlook_up_edu_ph/Documents/1 - EDUCATION/SCHOOLWORK/Undergraduate/Semester 6/CS 132/Machine Project/Solar-Wind-Energy-Analysis-Philippines/Data/WindPotential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C621C5F5-60A4-4E66-8C61-1A9A9E7B727A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C621C5F5-60A4-4E66-8C61-1A9A9E7B727A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEA2574A-6884-4302-8820-B062FB164152}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="2484" windowWidth="23040" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -690,13 +690,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>